<commit_message>
fix multiple markers bug; new feature: show nearest stations
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="March 5th" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -48,17 +48,34 @@
     <t>Replace mocking data with actual data to show fire stations' info when clicked.</t>
   </si>
   <si>
-    <t>Fix bug: The info window of previous marker doesn't close automatically when a nother marker is clicked.</t>
+    <t>Fix bug: Remove previous marker when another accident spot is clicked.</t>
+  </si>
+  <si>
+    <t>Fix bug: The info window of previous marker doesn't close automatically when another marker is clicked.</t>
+  </si>
+  <si>
+    <t>New feature: Show nearest k fire stations</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>New feature: Add custom control</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Fix bug: Restrict the map bounders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="m/d;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="166" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,29 +119,29 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,25 +423,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="96.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="18.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="96.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -439,39 +456,113 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>43895</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>0.625</v>
       </c>
+      <c r="F2" s="9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="4">
+        <v>43895</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43899</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7">
-        <v>0.625</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.63541666666666663</v>
+      <c r="D5" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.53125</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.53125</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new feature: Control Panel
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -60,13 +60,16 @@
     <t>3</t>
   </si>
   <si>
-    <t>New feature: Add custom control</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
     <t>Fix bug: Restrict the map bounders</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>New feature: Add custom control panel</t>
   </si>
 </sst>
 </file>
@@ -75,7 +78,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="166" formatCode="m/d;@"/>
+    <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -122,10 +125,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,27 +545,38 @@
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="6">
-        <v>0.57291666666666663</v>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.59375</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Feature: Test Case - Show k nearest nodes besides accident spot
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
-    <sheet name="March 5th" sheetId="1" r:id="rId1"/>
+    <sheet name="work" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Replace Accident Icon</t>
+  </si>
+  <si>
+    <t>New feature: Show nearest k nodes besides the accident spot.</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +508,6 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>43895</v>
-      </c>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -661,6 +661,26 @@
       </c>
       <c r="F12" s="9">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43901</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start generating combined JSON file
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C10799-E73A-4735-919E-AD76AC479F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7DEEEB-2839-4182-AB46-BD6273D61222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Fix bugs: duplicated info window</t>
+  </si>
+  <si>
+    <t>Change info window style</t>
+  </si>
+  <si>
+    <t>Generate the JSON file containing Up/Down Streams as well as intermediate points</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,6 +779,37 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>43911</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
read XML into POJO
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7DEEEB-2839-4182-AB46-BD6273D61222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED361317-B497-47A3-A635-A5E8E55334C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -112,7 +112,10 @@
     <t>Change info window style</t>
   </si>
   <si>
-    <t>Generate the JSON file containing Up/Down Streams as well as intermediate points</t>
+    <t>Read XML into POJO</t>
+  </si>
+  <si>
+    <t>Read XLSX into POJO</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
@@ -807,7 +810,27 @@
         <v>30</v>
       </c>
       <c r="D23" s="6">
-        <v>0.97222222222222221</v>
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E23" s="6">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F23" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>43912</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="6">
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read XLSX into POJO
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED361317-B497-47A3-A635-A5E8E55334C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D3CB15-C26E-428C-8A5F-458E7A7B1A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Read XLSX into POJO</t>
+  </si>
+  <si>
+    <t>Merge files</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,6 +835,23 @@
       <c r="D24" s="6">
         <v>6.25E-2</v>
       </c>
+      <c r="E24" s="6">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.14583333333333334</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
write JSON to file
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAC2677-ACC2-44A0-8AE9-6BE285A069DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127390D3-9F8C-40FB-9845-04F43E6FCC77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Find nearest Link to accident spot</t>
+  </si>
+  <si>
+    <t>Calculate sphere distance between two points, calculate distance between a point to a segment</t>
+  </si>
+  <si>
+    <t>Find nearest Link to accident spot - 2: Format path.json</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,6 +885,48 @@
         <v>2</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>43913</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F28" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
show circle and nodes inside
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127390D3-9F8C-40FB-9845-04F43E6FCC77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EF6D57-8A8F-4763-BD99-8F47C41D95AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Find nearest Link to accident spot - 2: Format path.json</t>
+  </si>
+  <si>
+    <t>Format node.json, Show nearest nodes inside circle.</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,6 +929,23 @@
       <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="C29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E29" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete looking for nearest path
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EF6D57-8A8F-4763-BD99-8F47C41D95AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC229DE6-D576-41D3-87A9-2F95E3859A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -130,7 +130,13 @@
     <t>Find nearest Link to accident spot - 2: Format path.json</t>
   </si>
   <si>
-    <t>Format node.json, Show nearest nodes inside circle.</t>
+    <t>Format paths.json</t>
+  </si>
+  <si>
+    <t>Format nodes.json, Show nearest nodes inside circle.</t>
+  </si>
+  <si>
+    <t>Find nearest path to accident spot</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,7 +936,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D29" s="6">
         <v>0.95833333333333337</v>
@@ -945,6 +951,35 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F30" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draw routes and intermedia point markers
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC229DE6-D576-41D3-87A9-2F95E3859A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C00515-7893-4D78-BA1D-74B37CE3F242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Find nearest path to accident spot</t>
+  </si>
+  <si>
+    <t>Draw the nearest path</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F16" sqref="F16:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,8 +952,11 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>43914</v>
+      </c>
       <c r="B30" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>36</v>
@@ -967,7 +973,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>38</v>
@@ -979,6 +985,23 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="F31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="F32" s="9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change sidebar click event
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B046C8E-845B-476D-BB20-D55F679852A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BDA996-6347-42C1-93D7-0B6EBC15C8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Click the sidebar interaction</t>
+  </si>
+  <si>
+    <t>Change click sidebar interaction</t>
   </si>
 </sst>
 </file>
@@ -502,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,8 +1055,25 @@
       <c r="B35" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="C35" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="D35" s="6">
-        <v>0.76388888888888884</v>
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.91666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add travel time and risk
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2296935-0829-40A9-871C-AEA083102259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865164D0-D234-45C5-A151-7A435F4D89EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>debug</t>
+  </si>
+  <si>
+    <t>Skype meeting with Hassan</t>
+  </si>
+  <si>
+    <t>Travel time and risk</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,6 +1143,43 @@
         <v>4</v>
       </c>
     </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>43923</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.65625</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F40" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
travel risk, sorting by time, badge
</commit_message>
<xml_diff>
--- a/doc/daily sheet.xlsx
+++ b/doc/daily sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865164D0-D234-45C5-A151-7A435F4D89EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24169781-E8B2-49EF-9AC3-D20006800D1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>JOB NO.</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Travel time and risk</t>
+  </si>
+  <si>
+    <t>Emails with Hassan and Dr.</t>
+  </si>
+  <si>
+    <t>Travel Risk : Low/Medium/High, Sort by travel time, shortest badge</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,6 +1186,43 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0.8125</v>
+      </c>
+      <c r="F41" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>43924</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="F42" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>